<commit_message>
Pequenas melhorias de textos e descrições.
Melhorado textos descrevendo as florestas.
Adicionado descrição às cidade-estado.
Adicionado mais duas linhas de textos de uma atualização silenciosa.
</commit_message>
<xml_diff>
--- a/PTBR/Lang/PTBR/Game/Faction.xlsx
+++ b/PTBR/Lang/PTBR/Game/Faction.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isy\Documents\GitHub\elin-portugues-brasileiro\Traduzido\PTBR\Lang\PTBR\Game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isy\Documents\GitHub\elin-portugues-brasileiro\PTBR\Lang\PTBR\Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4573251A-9731-4434-BC80-F6271D6D8F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACC5FF6-36EC-425F-B46B-83E715E91007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="540" windowWidth="20400" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Faction" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Casa</t>
   </si>
   <si>
-    <t>Selvageria</t>
-  </si>
-  <si>
     <t>Guilda dos Lutadores</t>
   </si>
   <si>
@@ -200,6 +197,45 @@
   </si>
   <si>
     <t>O Conselho</t>
+  </si>
+  <si>
+    <t>Terras Selvagens</t>
+  </si>
+  <si>
+    <t>Uma região inexplorada, onde a natureza reina e o perigo espreita.</t>
+  </si>
+  <si>
+    <t>Lar dos guerreiros que vivem pela espada e pelo combate.</t>
+  </si>
+  <si>
+    <t>Um refúgio sombrio para os que vivem nas sombras.</t>
+  </si>
+  <si>
+    <t>Centro arcano de estudo e poder mágico.</t>
+  </si>
+  <si>
+    <t>Onde riqueza e influência valem mais que espadas.</t>
+  </si>
+  <si>
+    <t>Uma vila pacata cercada por mistérios antigos.</t>
+  </si>
+  <si>
+    <t>Cidade ancestral marcada por segredos e magia esquecida.</t>
+  </si>
+  <si>
+    <t>Terras frias onde o vento carrega histórias de guerra.</t>
+  </si>
+  <si>
+    <t>A cúpula que governa com sabedoria... E interesses ocultos.</t>
+  </si>
+  <si>
+    <t>Coração do comércio e das intrigas políticas.</t>
+  </si>
+  <si>
+    <t>Uma floresta viva, berço dos espíritos e da antiga magia.</t>
+  </si>
+  <si>
+    <t>Sua base.</t>
   </si>
 </sst>
 </file>
@@ -240,9 +276,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,14 +620,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="16" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="11" width="16" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="55.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="11" width="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -642,8 +683,11 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -651,13 +695,16 @@
         <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -668,13 +715,16 @@
         <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -685,13 +735,16 @@
         <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -702,13 +755,16 @@
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -719,13 +775,16 @@
         <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
       </c>
       <c r="E8" t="s">
         <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -744,6 +803,9 @@
       <c r="E9" t="s">
         <v>31</v>
       </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -761,6 +823,9 @@
       <c r="E10" t="s">
         <v>34</v>
       </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -778,6 +843,9 @@
       <c r="E11" t="s">
         <v>37</v>
       </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -787,13 +855,16 @@
         <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
         <v>39</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -812,6 +883,9 @@
       <c r="E13" t="s">
         <v>43</v>
       </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -828,6 +902,9 @@
       </c>
       <c r="E14" t="s">
         <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>